<commit_message>
Fixed and passed failed test cases after introucing FirstPlayer & SecondPlayer properties and fixed the players always to TWO
</commit_message>
<xml_diff>
--- a/Documents/DataModel.xlsx
+++ b/Documents/DataModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Syed\Personal\Preperation\Tennis\Working\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356CA821-9443-4AE2-AC44-C1ED4E6BF4EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A425642-841D-4969-AA1D-F3CA353CCF0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,14 +388,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>